<commit_message>
checkpoint: improving implementation with rust
</commit_message>
<xml_diff>
--- a/test/sra_metadata.xlsx
+++ b/test/sra_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjpc/Documents/TESIS/MITNANEX_PROJECT/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D23665F-DAC4-D24D-97D7-A2574097EEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FD726D-D563-9546-BF1B-A16CE8A908BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>